<commit_message>
More 10 Finishing up 8
</commit_message>
<xml_diff>
--- a/Protokoll 10/Versuch 70 Berechnungen.xlsx
+++ b/Protokoll 10/Versuch 70 Berechnungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="540" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>80 mm</t>
   </si>
@@ -68,6 +68,60 @@
   <si>
     <t>error</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>delta s</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>dfds</t>
+  </si>
+  <si>
+    <t>dfde</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>80 -200</t>
+  </si>
+  <si>
+    <t>x_schirm</t>
+  </si>
+  <si>
+    <t>x_linse</t>
+  </si>
+  <si>
+    <t>b'</t>
+  </si>
+  <si>
+    <t>g'</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>(1+1/beta)</t>
+  </si>
+  <si>
+    <t>(1+beta)</t>
+  </si>
+  <si>
+    <t>delta 1/beta</t>
+  </si>
 </sst>
 </file>
 
@@ -115,8 +169,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,7 +341,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -269,6 +391,40 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -318,6 +474,40 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U21"/>
+  <dimension ref="B2:AF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17:U21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -659,7 +849,7 @@
     <col min="21" max="21" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:32">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -702,8 +892,29 @@
       <c r="R2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:21">
+      <c r="W2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32">
       <c r="C3">
         <v>67.8</v>
       </c>
@@ -764,8 +975,40 @@
         <f>(0.2/K3)*P3</f>
         <v>8.3982800322493969E-5</v>
       </c>
-    </row>
-    <row r="4" spans="2:21">
+      <c r="W3">
+        <f>C3-D3</f>
+        <v>57.699999999999996</v>
+      </c>
+      <c r="X3">
+        <f>SQRT(0.2^2+0.2^2)</f>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y3">
+        <f>F3-E3</f>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="Z3">
+        <f>SQRT(0.2^2+0.2^2)</f>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB3">
+        <f>(W3^2-Y3^2)/(4*W3)</f>
+        <v>7.7331022530329285</v>
+      </c>
+      <c r="AD3">
+        <f>(W3^2+Y3^2)/(4*W3^2)</f>
+        <v>0.36597743062334609</v>
+      </c>
+      <c r="AE3">
+        <f>Y3/(2*W3)</f>
+        <v>0.34055459272097055</v>
+      </c>
+      <c r="AF3">
+        <f>SQRT((AD3*X3)^2+(AE3*Z3)^2)</f>
+        <v>0.14139785298200602</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32">
       <c r="C4">
         <v>82.5</v>
       </c>
@@ -779,7 +1022,7 @@
         <v>73.400000000000006</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H22" si="0">C4-E4</f>
+        <f t="shared" ref="H4:H21" si="0">C4-E4</f>
         <v>63.5</v>
       </c>
       <c r="I4">
@@ -826,8 +1069,40 @@
         <f t="shared" ref="U4:U21" si="11">(0.2/K4)*P4</f>
         <v>4.9914023095218483E-5</v>
       </c>
-    </row>
-    <row r="5" spans="2:21">
+      <c r="W4">
+        <f t="shared" ref="W4:W21" si="12">C4-D4</f>
+        <v>72.400000000000006</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X21" si="13">SQRT(0.2^2+0.2^2)</f>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y21" si="14">F4-E4</f>
+        <v>54.400000000000006</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z21" si="15">SQRT(0.2^2+0.2^2)</f>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" ref="AB4:AB21" si="16">(W4^2-Y4^2)/(4*W4)</f>
+        <v>7.8812154696132612</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD21" si="17">(W4^2+Y4^2)/(4*W4^2)</f>
+        <v>0.3911434327401484</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" ref="AE4:AE21" si="18">Y4/(2*W4)</f>
+        <v>0.37569060773480661</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF21" si="19">SQRT((AD4*X4)^2+(AE4*Z4)^2)</f>
+        <v>0.15339794463183537</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32">
       <c r="C5">
         <v>98.8</v>
       </c>
@@ -888,8 +1163,40 @@
         <f t="shared" si="11"/>
         <v>3.1644317867172983E-5</v>
       </c>
-    </row>
-    <row r="6" spans="2:21">
+      <c r="W5">
+        <f t="shared" si="12"/>
+        <v>88.7</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="14"/>
+        <v>70.8</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="16"/>
+        <v>8.0469278466741851</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="17"/>
+        <v>0.4092792801953305</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="18"/>
+        <v>0.39909808342728292</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="19"/>
+        <v>0.16168829503524082</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32">
       <c r="C6">
         <v>116.5</v>
       </c>
@@ -950,8 +1257,40 @@
         <f t="shared" si="11"/>
         <v>2.1038790269559499E-5</v>
       </c>
-    </row>
-    <row r="7" spans="2:21">
+      <c r="W6">
+        <f t="shared" si="12"/>
+        <v>106.4</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="14"/>
+        <v>89.199999999999989</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="16"/>
+        <v>7.9048872180451202</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="17"/>
+        <v>0.42570594719882404</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="18"/>
+        <v>0.41917293233082698</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="19"/>
+        <v>0.16898082747560972</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32">
       <c r="C7">
         <v>77.8</v>
       </c>
@@ -1012,8 +1351,40 @@
         <f t="shared" si="11"/>
         <v>5.9045122282448261E-5</v>
       </c>
-    </row>
-    <row r="8" spans="2:21">
+      <c r="W7">
+        <f t="shared" si="12"/>
+        <v>67.7</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="14"/>
+        <v>48.9</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="16"/>
+        <v>8.0948301329394372</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="17"/>
+        <v>0.38043086952822097</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="18"/>
+        <v>0.36115214180206789</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="19"/>
+        <v>0.14836671217445491</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32">
       <c r="H8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1062,8 +1433,44 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="2:21">
+      <c r="W8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB8">
+        <f>AVERAGE(AB3:AB7)</f>
+        <v>7.9321925840609868</v>
+      </c>
+      <c r="AC8">
+        <f>STDEV(AB3:AB7)</f>
+        <v>0.14369791396506831</v>
+      </c>
+      <c r="AD8" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE8" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF8" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -1115,8 +1522,40 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="2:21">
+      <c r="W9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB9" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD9" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE9" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF9" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32">
       <c r="C10">
         <v>77.8</v>
       </c>
@@ -1177,8 +1616,40 @@
         <f t="shared" si="11"/>
         <v>5.0873886179854466E-5</v>
       </c>
-    </row>
-    <row r="11" spans="2:21">
+      <c r="W10">
+        <f t="shared" si="12"/>
+        <v>67.7</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="14"/>
+        <v>55.3</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="16"/>
+        <v>5.6322008862629254</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="17"/>
+        <v>0.41680648617041466</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="18"/>
+        <v>0.40841949778434267</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="19"/>
+        <v>0.16505372048739594</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32">
       <c r="C11">
         <v>94</v>
       </c>
@@ -1239,8 +1710,40 @@
         <f t="shared" si="11"/>
         <v>3.2046146450889282E-5</v>
       </c>
-    </row>
-    <row r="12" spans="2:21">
+      <c r="W11">
+        <f t="shared" si="12"/>
+        <v>83.9</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="14"/>
+        <v>71.8</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="16"/>
+        <v>5.613736591179979</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="17"/>
+        <v>0.43309014790011946</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="18"/>
+        <v>0.42789034564958278</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="19"/>
+        <v>0.17219923904785803</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32">
       <c r="C12">
         <v>44.2</v>
       </c>
@@ -1301,8 +1804,40 @@
         <f t="shared" si="11"/>
         <v>2.6065763922376162E-4</v>
       </c>
-    </row>
-    <row r="13" spans="2:21">
+      <c r="W12">
+        <f t="shared" si="12"/>
+        <v>34.1</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="14"/>
+        <v>19.499999999999996</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="16"/>
+        <v>5.7372434017595326</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="17"/>
+        <v>0.33175239291027764</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="18"/>
+        <v>0.28592375366568906</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="19"/>
+        <v>0.12387478940025624</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32">
       <c r="C13">
         <v>34.1</v>
       </c>
@@ -1363,8 +1898,40 @@
         <f t="shared" si="11"/>
         <v>8.0115366127223215E-4</v>
       </c>
-    </row>
-    <row r="14" spans="2:21">
+      <c r="W13">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="14"/>
+        <v>5.8999999999999986</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="16"/>
+        <v>5.6373958333333336</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="17"/>
+        <v>0.26510850694444443</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="18"/>
+        <v>0.12291666666666663</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="19"/>
+        <v>8.265157101895014E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32">
       <c r="C14">
         <v>49.1</v>
       </c>
@@ -1425,8 +1992,40 @@
         <f t="shared" si="11"/>
         <v>1.7928215425436553E-4</v>
       </c>
-    </row>
-    <row r="15" spans="2:21">
+      <c r="W14">
+        <f t="shared" si="12"/>
+        <v>39</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="14"/>
+        <v>25.6</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="16"/>
+        <v>5.5489743589743581</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="17"/>
+        <v>0.35771860618014467</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="18"/>
+        <v>0.3282051282051282</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="19"/>
+        <v>0.13731167681959469</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32">
       <c r="H15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1475,8 +2074,44 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="2:21">
+      <c r="W15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB15">
+        <f>AVERAGE(AB10:AB14)</f>
+        <v>5.6339102143020252</v>
+      </c>
+      <c r="AC15">
+        <f>STDEV(AB10:AB14)</f>
+        <v>6.7664417463349599E-2</v>
+      </c>
+      <c r="AD15" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE15" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF15" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32">
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -1528,8 +2163,40 @@
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="17" spans="3:21">
+      <c r="W16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB16" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD16" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AE16" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF16" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32">
       <c r="C17">
         <v>105.8</v>
       </c>
@@ -1590,8 +2257,40 @@
         <f t="shared" si="11"/>
         <v>2.7746909341135758E-5</v>
       </c>
-    </row>
-    <row r="18" spans="3:21">
+      <c r="W17">
+        <f t="shared" si="12"/>
+        <v>95.7</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="14"/>
+        <v>68.599999999999994</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="16"/>
+        <v>11.631478578892374</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="17"/>
+        <v>0.37845894901888849</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="18"/>
+        <v>0.35841170323928939</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" si="19"/>
+        <v>0.14742866074447539</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32">
       <c r="C18">
         <v>84.9</v>
       </c>
@@ -1652,8 +2351,40 @@
         <f t="shared" si="11"/>
         <v>5.007210382951451E-5</v>
       </c>
-    </row>
-    <row r="19" spans="3:21">
+      <c r="W18">
+        <f t="shared" si="12"/>
+        <v>74.800000000000011</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="14"/>
+        <v>46.199999999999996</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="16"/>
+        <v>11.566176470588241</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="17"/>
+        <v>0.34537197231833905</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="18"/>
+        <v>0.30882352941176461</v>
+      </c>
+      <c r="AF18">
+        <f t="shared" si="19"/>
+        <v>0.13104312926098755</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32">
       <c r="C19">
         <v>130.80000000000001</v>
       </c>
@@ -1714,8 +2445,40 @@
         <f t="shared" si="11"/>
         <v>1.6350074719841467E-5</v>
       </c>
-    </row>
-    <row r="20" spans="3:21">
+      <c r="W19">
+        <f t="shared" si="12"/>
+        <v>120.70000000000002</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="14"/>
+        <v>94.9</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="16"/>
+        <v>11.521292460646235</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="17"/>
+        <v>0.40454604423656809</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="18"/>
+        <v>0.39312344656172327</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="19"/>
+        <v>0.15955025443891302</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32">
       <c r="C20">
         <v>69.7</v>
       </c>
@@ -1776,8 +2539,40 @@
         <f t="shared" si="11"/>
         <v>9.1705679791277892E-5</v>
       </c>
-    </row>
-    <row r="21" spans="3:21">
+      <c r="W20">
+        <f t="shared" si="12"/>
+        <v>59.6</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="14"/>
+        <v>28.199999999999996</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="16"/>
+        <v>11.564261744966444</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="17"/>
+        <v>0.30596876266834822</v>
+      </c>
+      <c r="AE20">
+        <f t="shared" si="18"/>
+        <v>0.23657718120805366</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="19"/>
+        <v>0.10939310632654996</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32">
       <c r="C21">
         <v>61.4</v>
       </c>
@@ -1837,6 +2632,1037 @@
       <c r="U21">
         <f t="shared" si="11"/>
         <v>1.5432098765432098E-4</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="12"/>
+        <v>51.3</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="13"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="14"/>
+        <v>15.5</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="15"/>
+        <v>0.28284271247461906</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="16"/>
+        <v>11.6541910331384</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="17"/>
+        <v>0.27282278687839373</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="18"/>
+        <v>0.1510721247563353</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="19"/>
+        <v>8.8206602890480809E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32">
+      <c r="AB22">
+        <f>AVERAGE(AB17:AB21)</f>
+        <v>11.58748005764634</v>
+      </c>
+      <c r="AC22">
+        <f>STDEV(AB17:AB21)</f>
+        <v>5.4221663071210735E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" t="s">
+        <v>31</v>
+      </c>
+      <c r="N25" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32">
+      <c r="C26">
+        <v>76.5</v>
+      </c>
+      <c r="D26">
+        <v>28.6</v>
+      </c>
+      <c r="E26">
+        <f>D26-10.1</f>
+        <v>18.5</v>
+      </c>
+      <c r="F26">
+        <f>C26-D26</f>
+        <v>47.9</v>
+      </c>
+      <c r="H26">
+        <v>2.1</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="J26">
+        <f>I26/H26</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="K26">
+        <f>(0.1/I26)*J26</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="M26">
+        <f>1+(1/J26)</f>
+        <v>1.3</v>
+      </c>
+      <c r="N26">
+        <f>1+J26</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="O26">
+        <f>(K26/J26)*M26</f>
+        <v>1.8571428571428572E-2</v>
+      </c>
+      <c r="Q26">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32">
+      <c r="C27">
+        <v>59.5</v>
+      </c>
+      <c r="D27">
+        <v>30.9</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27:E46" si="20">D27-10.1</f>
+        <v>20.799999999999997</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F46" si="21">C27-D27</f>
+        <v>28.6</v>
+      </c>
+      <c r="H27">
+        <v>2.1</v>
+      </c>
+      <c r="I27">
+        <v>3.6</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J46" si="22">I27/H27</f>
+        <v>1.7142857142857142</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:K46" si="23">(0.1/I27)*J27</f>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M46" si="24">1+(1/J27)</f>
+        <v>1.5833333333333335</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ref="N27:N46" si="25">1+J27</f>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ref="O27:O46" si="26">(K27/J27)*M27</f>
+        <v>4.3981481481481483E-2</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ref="Q27:Q46" si="27">0.2</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32">
+      <c r="C28">
+        <v>54.8</v>
+      </c>
+      <c r="D28">
+        <v>29.8</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="20"/>
+        <v>19.700000000000003</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="21"/>
+        <v>24.999999999999996</v>
+      </c>
+      <c r="H28">
+        <v>2.1</v>
+      </c>
+      <c r="I28">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="22"/>
+        <v>2.1904761904761902</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="23"/>
+        <v>4.7619047619047623E-2</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="24"/>
+        <v>1.4565217391304348</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="25"/>
+        <v>3.1904761904761902</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="26"/>
+        <v>3.1663516068052934E-2</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32">
+      <c r="C29">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="D29">
+        <v>27.9</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="20"/>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="21"/>
+        <v>47.199999999999996</v>
+      </c>
+      <c r="H29">
+        <v>2.1</v>
+      </c>
+      <c r="I29">
+        <v>7.8</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="22"/>
+        <v>3.714285714285714</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="23"/>
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="24"/>
+        <v>1.2692307692307692</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="25"/>
+        <v>4.7142857142857135</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="26"/>
+        <v>1.6272189349112426E-2</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32">
+      <c r="C30">
+        <v>100.1</v>
+      </c>
+      <c r="D30">
+        <v>25.4</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="20"/>
+        <v>15.299999999999999</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="21"/>
+        <v>74.699999999999989</v>
+      </c>
+      <c r="H30">
+        <v>0.7</v>
+      </c>
+      <c r="I30">
+        <v>3.3</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="22"/>
+        <v>4.7142857142857144</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="24"/>
+        <v>1.2121212121212122</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="25"/>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="26"/>
+        <v>3.6730945821854918E-2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32">
+      <c r="C31">
+        <v>116.5</v>
+      </c>
+      <c r="D31">
+        <v>26.2</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="20"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="21"/>
+        <v>90.3</v>
+      </c>
+      <c r="H31">
+        <v>0.7</v>
+      </c>
+      <c r="I31">
+        <v>4.7</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="22"/>
+        <v>6.7142857142857153</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="24"/>
+        <v>1.1489361702127658</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="25"/>
+        <v>7.7142857142857153</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="26"/>
+        <v>2.4445450430058847E-2</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32">
+      <c r="C32">
+        <v>127.9</v>
+      </c>
+      <c r="D32">
+        <v>26.1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="21"/>
+        <v>101.80000000000001</v>
+      </c>
+      <c r="H32">
+        <v>0.7</v>
+      </c>
+      <c r="I32">
+        <v>5.5</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="22"/>
+        <v>7.8571428571428577</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="24"/>
+        <v>1.1272727272727272</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="25"/>
+        <v>8.8571428571428577</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="26"/>
+        <v>2.0495867768595043E-2</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17">
+      <c r="C33">
+        <v>82</v>
+      </c>
+      <c r="D33">
+        <v>27.4</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="20"/>
+        <v>17.299999999999997</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="21"/>
+        <v>54.6</v>
+      </c>
+      <c r="H33">
+        <v>1.4</v>
+      </c>
+      <c r="I33">
+        <v>5.3</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="22"/>
+        <v>3.785714285714286</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="24"/>
+        <v>1.2641509433962264</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="25"/>
+        <v>4.7857142857142865</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="26"/>
+        <v>2.3851904592381633E-2</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17">
+      <c r="C34">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D34">
+        <v>28.4</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="20"/>
+        <v>18.299999999999997</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="21"/>
+        <v>41.699999999999996</v>
+      </c>
+      <c r="H34">
+        <v>1.4</v>
+      </c>
+      <c r="I34">
+        <v>3.8</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="22"/>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="24"/>
+        <v>1.368421052631579</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="25"/>
+        <v>3.7142857142857144</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="26"/>
+        <v>3.6011080332409975E-2</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17">
+      <c r="C35">
+        <v>67.5</v>
+      </c>
+      <c r="D35">
+        <v>28.5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="20"/>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="21"/>
+        <v>39</v>
+      </c>
+      <c r="H35">
+        <v>0.7</v>
+      </c>
+      <c r="I35">
+        <v>1.8</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="22"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="24"/>
+        <v>1.3888888888888888</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="25"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="26"/>
+        <v>7.716049382716049E-2</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17">
+      <c r="E36">
+        <f>D36-10.1</f>
+        <v>-10.1</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J36" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K36" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N36" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O36" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
+      <c r="C37">
+        <v>82.2</v>
+      </c>
+      <c r="D37">
+        <v>23.6</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="20"/>
+        <v>13.500000000000002</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="21"/>
+        <v>58.6</v>
+      </c>
+      <c r="H37">
+        <v>0.7</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="22"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="24"/>
+        <v>1.35</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="25"/>
+        <v>3.8571428571428572</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="26"/>
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17">
+      <c r="C38">
+        <v>75.5</v>
+      </c>
+      <c r="D38">
+        <v>24</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="20"/>
+        <v>13.9</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="21"/>
+        <v>51.5</v>
+      </c>
+      <c r="H38">
+        <v>1.4</v>
+      </c>
+      <c r="I38">
+        <v>4.5</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="22"/>
+        <v>3.2142857142857144</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="24"/>
+        <v>1.3111111111111111</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="25"/>
+        <v>4.2142857142857144</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="26"/>
+        <v>2.9135802469135802E-2</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17">
+      <c r="C39">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>24.7</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="20"/>
+        <v>14.6</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="21"/>
+        <v>44.3</v>
+      </c>
+      <c r="H39">
+        <v>1.4</v>
+      </c>
+      <c r="I39">
+        <v>3.7</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="22"/>
+        <v>2.6428571428571432</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="24"/>
+        <v>1.3783783783783783</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="25"/>
+        <v>3.6428571428571432</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="26"/>
+        <v>3.7253469685902117E-2</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:17">
+      <c r="C40">
+        <v>56.8</v>
+      </c>
+      <c r="D40">
+        <v>31.5</v>
+      </c>
+      <c r="E40">
+        <f>D40-10.1</f>
+        <v>21.4</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="21"/>
+        <v>25.299999999999997</v>
+      </c>
+      <c r="H40">
+        <v>1.4</v>
+      </c>
+      <c r="I40">
+        <v>1.4</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="26"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17">
+      <c r="C41">
+        <v>116.1</v>
+      </c>
+      <c r="D41">
+        <v>22.5</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="20"/>
+        <v>12.4</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="21"/>
+        <v>93.6</v>
+      </c>
+      <c r="H41">
+        <v>0.7</v>
+      </c>
+      <c r="I41">
+        <v>4.8</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="22"/>
+        <v>6.8571428571428577</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="24"/>
+        <v>1.1458333333333333</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="25"/>
+        <v>7.8571428571428577</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="26"/>
+        <v>2.387152777777778E-2</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17">
+      <c r="C42">
+        <v>107</v>
+      </c>
+      <c r="D42">
+        <v>22.5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="20"/>
+        <v>12.4</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="21"/>
+        <v>84.5</v>
+      </c>
+      <c r="H42">
+        <v>0.7</v>
+      </c>
+      <c r="I42">
+        <v>4.3</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="22"/>
+        <v>6.1428571428571432</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="24"/>
+        <v>1.1627906976744187</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="25"/>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="26"/>
+        <v>2.7041644131963229E-2</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:17">
+      <c r="C43">
+        <v>130.69999999999999</v>
+      </c>
+      <c r="D43">
+        <v>22.1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="20"/>
+        <v>12.000000000000002</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="21"/>
+        <v>108.6</v>
+      </c>
+      <c r="H43">
+        <v>0.7</v>
+      </c>
+      <c r="I43">
+        <v>5.7</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="22"/>
+        <v>8.1428571428571441</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="24"/>
+        <v>1.1228070175438596</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="25"/>
+        <v>9.1428571428571441</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="26"/>
+        <v>1.9698368728839642E-2</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17">
+      <c r="C44">
+        <v>99</v>
+      </c>
+      <c r="D44">
+        <v>23</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="20"/>
+        <v>12.9</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="21"/>
+        <v>76</v>
+      </c>
+      <c r="H44">
+        <v>0.7</v>
+      </c>
+      <c r="I44">
+        <v>5.6</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="22"/>
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="23"/>
+        <v>0.14285714285714288</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="24"/>
+        <v>1.125</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="25"/>
+        <v>9</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="26"/>
+        <v>2.0089285714285716E-2</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:17">
+      <c r="C45">
+        <v>91.5</v>
+      </c>
+      <c r="D45">
+        <v>22.9</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="20"/>
+        <v>12.799999999999999</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="21"/>
+        <v>68.599999999999994</v>
+      </c>
+      <c r="H45">
+        <v>1.4</v>
+      </c>
+      <c r="I45">
+        <v>6.5</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="22"/>
+        <v>4.6428571428571432</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="24"/>
+        <v>1.2153846153846153</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="25"/>
+        <v>5.6428571428571432</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="26"/>
+        <v>1.8698224852071007E-2</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:17">
+      <c r="C46">
+        <v>73</v>
+      </c>
+      <c r="D46">
+        <v>24.4</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="20"/>
+        <v>14.299999999999999</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="21"/>
+        <v>48.6</v>
+      </c>
+      <c r="H46">
+        <v>1.4</v>
+      </c>
+      <c r="I46">
+        <v>4.2</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="22"/>
+        <v>3.0000000000000004</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="23"/>
+        <v>7.1428571428571438E-2</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="24"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="26"/>
+        <v>3.1746031746031744E-2</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="27"/>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>